<commit_message>
Another step on Excel program
</commit_message>
<xml_diff>
--- a/Excel Esports Sequencing Leeloo - old.xlsx
+++ b/Excel Esports Sequencing Leeloo - old.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325EA2F9-15EF-4FEA-8BA4-468A874C1120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9CC118-804F-4690-918A-1696297B8C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="1104">
   <si>
     <t>Test Case</t>
   </si>
@@ -6266,6 +6266,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6281,21 +6296,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6324,9 +6324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1655054</xdr:colOff>
+      <xdr:colOff>1123559</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>129629</xdr:rowOff>
+      <xdr:rowOff>133439</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6683,8 +6683,8 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120:E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -6698,7 +6698,8 @@
     <col min="7" max="7" width="27.09765625" customWidth="1"/>
     <col min="8" max="8" width="91.69921875" customWidth="1"/>
     <col min="9" max="9" width="6.296875" customWidth="1"/>
-    <col min="10" max="11" width="11.3984375" customWidth="1"/>
+    <col min="10" max="10" width="11.3984375" customWidth="1"/>
+    <col min="11" max="11" width="18.19921875" customWidth="1"/>
     <col min="12" max="12" width="83.09765625" customWidth="1"/>
     <col min="13" max="13" width="81.3984375" customWidth="1"/>
     <col min="14" max="14" width="7.69921875" customWidth="1"/>
@@ -7195,7 +7196,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="160">
         <f t="array" ref="J30">SUMPRODUCT(--($F$23:$F$242=1),$D$23:$D$242)</f>
-        <v>220</v>
+        <v>360</v>
       </c>
       <c r="K30" s="161"/>
       <c r="L30" s="1"/>
@@ -8366,7 +8367,7 @@
         <v>10000</v>
       </c>
       <c r="Q86" t="e" vm="2">
-        <f t="shared" ref="Q86:Q88" si="5">MID(M86,P86,P86+2)</f>
+        <f t="shared" ref="Q86" si="5">MID(M86,P86,P86+2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="S86" t="e" cm="1" vm="2">
@@ -8484,7 +8485,7 @@
         <v>CTG</v>
       </c>
       <c r="L89" s="157" t="e" vm="7">
-        <f t="shared" ref="L87:L93" si="8">MID(H89,1,K89-1)</f>
+        <f t="shared" ref="L89:L93" si="8">MID(H89,1,K89-1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="M89" t="e" cm="1" vm="2">
@@ -8496,7 +8497,7 @@
         <v>10000</v>
       </c>
       <c r="Q89" t="e" vm="2">
-        <f t="shared" ref="Q87:Q93" si="9">MID(M89,P89,P89+2)</f>
+        <f t="shared" ref="Q89:Q93" si="9">MID(M89,P89,P89+2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="S89" t="e" cm="1" vm="2">
@@ -9107,6 +9108,12 @@
       <c r="F109" s="10"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
+      <c r="J109" s="156" t="s">
+        <v>31</v>
+      </c>
+      <c r="K109" s="156" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="110" spans="1:11" ht="24.75" customHeight="1">
       <c r="A110" s="1"/>
@@ -9123,6 +9130,12 @@
       <c r="F110" s="10"/>
       <c r="G110" s="166"/>
       <c r="H110" s="167"/>
+      <c r="J110" s="156" t="s">
+        <v>37</v>
+      </c>
+      <c r="K110" s="156" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="111" spans="1:11" ht="14.25" customHeight="1">
       <c r="A111" s="1"/>
@@ -9133,6 +9146,12 @@
       <c r="F111" s="10"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
+      <c r="J111" s="156" t="s">
+        <v>33</v>
+      </c>
+      <c r="K111" s="156" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="112" spans="1:11" ht="14.25" customHeight="1">
       <c r="A112" s="1"/>
@@ -9145,8 +9164,14 @@
       <c r="F112" s="10"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-    </row>
-    <row r="113" spans="1:8" ht="14.25" customHeight="1">
+      <c r="J112" s="156" t="s">
+        <v>35</v>
+      </c>
+      <c r="K112" s="156" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="14.25" customHeight="1">
       <c r="A113" s="1"/>
       <c r="B113" s="3" t="s">
         <v>114</v>
@@ -9158,7 +9183,7 @@
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" spans="1:8" ht="14.25" customHeight="1">
+    <row r="114" spans="1:13" ht="14.25" customHeight="1">
       <c r="A114" s="1"/>
       <c r="B114" s="3"/>
       <c r="C114" s="2" t="s">
@@ -9170,7 +9195,7 @@
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
     </row>
-    <row r="115" spans="1:8" ht="15.75" customHeight="1">
+    <row r="115" spans="1:13" ht="15.75" customHeight="1">
       <c r="A115" s="1"/>
       <c r="B115" s="3"/>
       <c r="C115" s="4"/>
@@ -9180,7 +9205,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" ht="25.5" customHeight="1">
+    <row r="116" spans="1:13" ht="25.5" customHeight="1">
       <c r="A116" s="1"/>
       <c r="B116" s="5" t="s">
         <v>53</v>
@@ -9200,7 +9225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="15" customHeight="1">
+    <row r="117" spans="1:13" ht="15" customHeight="1">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -9210,7 +9235,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" ht="25.5" customHeight="1">
+    <row r="118" spans="1:13" ht="25.5" customHeight="1">
       <c r="A118" s="1"/>
       <c r="B118" s="11" t="s">
         <v>116</v>
@@ -9232,8 +9257,16 @@
       <c r="H118" s="25" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="15" customHeight="1">
+      <c r="K118" t="str" cm="1">
+        <f t="array" ref="K118">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H118,_xlfn.SEQUENCE(1,LEN(H118),LEN(H118),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CACCCCGAGATCACATTTCTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCC</v>
+      </c>
+      <c r="M118" t="str" cm="1">
+        <f t="array" ref="M118">MID(K118,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K118,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="15" customHeight="1">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -9242,8 +9275,16 @@
       <c r="F119" s="10"/>
       <c r="G119" s="1"/>
       <c r="H119" s="28"/>
-    </row>
-    <row r="120" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K119" t="e" cm="1" vm="4">
+        <f t="array" ref="K119">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H119,_xlfn.SEQUENCE(1,LEN(H119),LEN(H119),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M119" t="e" cm="1" vm="5">
+        <f t="array" ref="M119">MID(K119,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K119,4,999)),3)),3)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="25.5" customHeight="1">
       <c r="A120" s="1"/>
       <c r="B120" s="26">
         <f t="shared" ref="B120:B139" si="10">MAX($B$1:B119)+1</f>
@@ -9255,17 +9296,27 @@
       <c r="D120" s="12">
         <v>7</v>
       </c>
-      <c r="E120" s="34"/>
+      <c r="E120" s="34" t="s">
+        <v>1086</v>
+      </c>
       <c r="F120" s="10">
         <f>IF(ISBLANK(E120),0,IF(E120=Answers!E120,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120" s="1"/>
       <c r="H120" s="25" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K120" t="str" cm="1">
+        <f t="array" ref="K120">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H120,_xlfn.SEQUENCE(1,LEN(H120),LEN(H120),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>ATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACAGCTGCCTCCCCAACAGTGCATCCCCTTCTCCTTCCTCAGCCTCAGGTAGGAGACA</v>
+      </c>
+      <c r="M120" t="str" cm="1">
+        <f t="array" ref="M120">MID(K120,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K120,4,999)),3)),3)</f>
+        <v>GGC</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="25.5" customHeight="1">
       <c r="A121" s="1"/>
       <c r="B121" s="26">
         <f t="shared" si="10"/>
@@ -9277,17 +9328,27 @@
       <c r="D121" s="12">
         <v>7</v>
       </c>
-      <c r="E121" s="34"/>
+      <c r="E121" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F121" s="10">
         <f>IF(ISBLANK(E121),0,IF(E121=Answers!E121,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" s="1"/>
       <c r="H121" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K121" t="str" cm="1">
+        <f t="array" ref="K121">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H121,_xlfn.SEQUENCE(1,LEN(H121),LEN(H121),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>TCACTGGTCCAGGAGCACTATGCTGGCAGAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACAGCTGCCTCC</v>
+      </c>
+      <c r="M121" t="str" cm="1">
+        <f t="array" ref="M121">MID(K121,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K121,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="25.5" customHeight="1">
       <c r="A122" s="1"/>
       <c r="B122" s="26">
         <f t="shared" si="10"/>
@@ -9299,17 +9360,27 @@
       <c r="D122" s="12">
         <v>7</v>
       </c>
-      <c r="E122" s="34"/>
+      <c r="E122" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F122" s="10">
         <f>IF(ISBLANK(E122),0,IF(E122=Answers!E122,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="25" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K122" t="str" cm="1">
+        <f t="array" ref="K122">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H122,_xlfn.SEQUENCE(1,LEN(H122),LEN(H122),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACAGCTGCCTCCCCAACAGTGCATCCCCTTCTCCTTCCTC</v>
+      </c>
+      <c r="M122" t="str" cm="1">
+        <f t="array" ref="M122">MID(K122,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K122,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="25.5" customHeight="1">
       <c r="A123" s="1"/>
       <c r="B123" s="26">
         <f t="shared" si="10"/>
@@ -9321,17 +9392,27 @@
       <c r="D123" s="12">
         <v>7</v>
       </c>
-      <c r="E123" s="34"/>
+      <c r="E123" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F123" s="10">
         <f>IF(ISBLANK(E123),0,IF(E123=Answers!E123,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="25" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K123" t="str" cm="1">
+        <f t="array" ref="K123">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H123,_xlfn.SEQUENCE(1,LEN(H123),LEN(H123),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CGAGATCACATTTCTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCC</v>
+      </c>
+      <c r="M123" t="str" cm="1">
+        <f t="array" ref="M123">MID(K123,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K123,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="25.5" customHeight="1">
       <c r="A124" s="1"/>
       <c r="B124" s="26">
         <f t="shared" si="10"/>
@@ -9343,17 +9424,27 @@
       <c r="D124" s="12">
         <v>7</v>
       </c>
-      <c r="E124" s="34"/>
+      <c r="E124" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F124" s="10">
         <f>IF(ISBLANK(E124),0,IF(E124=Answers!E124,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="25" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K124" t="str" cm="1">
+        <f t="array" ref="K124">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H124,_xlfn.SEQUENCE(1,LEN(H124),LEN(H124),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GCAAAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCTGCCTGTCAGGAAGAGGCCTACTTCTGGTGAAACTGGGCAGACAAAAGGCAGTGAGAAATGTGA</v>
+      </c>
+      <c r="M124" t="str" cm="1">
+        <f t="array" ref="M124">MID(K124,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K124,4,999)),3)),3)</f>
+        <v>TGG</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="25.5" customHeight="1">
       <c r="A125" s="1"/>
       <c r="B125" s="26">
         <f t="shared" si="10"/>
@@ -9365,17 +9456,27 @@
       <c r="D125" s="12">
         <v>7</v>
       </c>
-      <c r="E125" s="34"/>
+      <c r="E125" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F125" s="10">
         <f>IF(ISBLANK(E125),0,IF(E125=Answers!E125,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="25" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K125" t="str" cm="1">
+        <f t="array" ref="K125">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H125,_xlfn.SEQUENCE(1,LEN(H125),LEN(H125),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>AGATCACATTTCTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCCTT</v>
+      </c>
+      <c r="M125" t="str" cm="1">
+        <f t="array" ref="M125">MID(K125,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K125,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="25.5" customHeight="1">
       <c r="A126" s="1"/>
       <c r="B126" s="26">
         <f t="shared" si="10"/>
@@ -9387,17 +9488,27 @@
       <c r="D126" s="12">
         <v>7</v>
       </c>
-      <c r="E126" s="34"/>
+      <c r="E126" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F126" s="10">
         <f>IF(ISBLANK(E126),0,IF(E126=Answers!E126,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" s="1"/>
       <c r="H126" s="25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K126" t="str" cm="1">
+        <f t="array" ref="K126">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H126,_xlfn.SEQUENCE(1,LEN(H126),LEN(H126),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GATCACATTTCTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCCTTT</v>
+      </c>
+      <c r="M126" t="str" cm="1">
+        <f t="array" ref="M126">MID(K126,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K126,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="25.5" customHeight="1">
       <c r="A127" s="1"/>
       <c r="B127" s="26">
         <f t="shared" si="10"/>
@@ -9409,17 +9520,27 @@
       <c r="D127" s="12">
         <v>7</v>
       </c>
-      <c r="E127" s="34"/>
+      <c r="E127" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F127" s="10">
         <f>IF(ISBLANK(E127),0,IF(E127=Answers!E127,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" s="25" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K127" t="str" cm="1">
+        <f t="array" ref="K127">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H127,_xlfn.SEQUENCE(1,LEN(H127),LEN(H127),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>ATCACATTTCTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCCTTTG</v>
+      </c>
+      <c r="M127" t="str" cm="1">
+        <f t="array" ref="M127">MID(K127,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K127,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="25.5" customHeight="1">
       <c r="A128" s="1"/>
       <c r="B128" s="26">
         <f t="shared" si="10"/>
@@ -9431,17 +9552,27 @@
       <c r="D128" s="12">
         <v>7</v>
       </c>
-      <c r="E128" s="34"/>
+      <c r="E128" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F128" s="10">
         <f>IF(ISBLANK(E128),0,IF(E128=Answers!E128,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K128" t="str" cm="1">
+        <f t="array" ref="K128">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H128,_xlfn.SEQUENCE(1,LEN(H128),LEN(H128),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GCATGTCCAGGACAGGGTGCCGGGTGTATCACTGGTCCAGGAGCACTATGCTGGCAGAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAG</v>
+      </c>
+      <c r="M128" t="str" cm="1">
+        <f t="array" ref="M128">MID(K128,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K128,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="25.5" customHeight="1">
       <c r="A129" s="1"/>
       <c r="B129" s="26">
         <f t="shared" si="10"/>
@@ -9453,17 +9584,27 @@
       <c r="D129" s="12">
         <v>7</v>
       </c>
-      <c r="E129" s="34"/>
+      <c r="E129" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F129" s="10">
         <f>IF(ISBLANK(E129),0,IF(E129=Answers!E129,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="25" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K129" t="str" cm="1">
+        <f t="array" ref="K129">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H129,_xlfn.SEQUENCE(1,LEN(H129),LEN(H129),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CCGGGTGTATCACTGGTCCAGGAGCACTATGCTGGCAGAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACA</v>
+      </c>
+      <c r="M129" t="str" cm="1">
+        <f t="array" ref="M129">MID(K129,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K129,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="25.5" customHeight="1">
       <c r="A130" s="1"/>
       <c r="B130" s="26">
         <f t="shared" si="10"/>
@@ -9475,17 +9616,27 @@
       <c r="D130" s="12">
         <v>7</v>
       </c>
-      <c r="E130" s="34"/>
+      <c r="E130" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F130" s="10">
         <f>IF(ISBLANK(E130),0,IF(E130=Answers!E130,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K130" t="str" cm="1">
+        <f t="array" ref="K130">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H130,_xlfn.SEQUENCE(1,LEN(H130),LEN(H130),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>TCCAGGAGCACTATGCTGGCAGAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACAGCTGCCTCCCCAACAG</v>
+      </c>
+      <c r="M130" t="str" cm="1">
+        <f t="array" ref="M130">MID(K130,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K130,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="25.5" customHeight="1">
       <c r="A131" s="1"/>
       <c r="B131" s="26">
         <f t="shared" si="10"/>
@@ -9497,17 +9648,27 @@
       <c r="D131" s="12">
         <v>7</v>
       </c>
-      <c r="E131" s="34"/>
+      <c r="E131" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F131" s="10">
         <f>IF(ISBLANK(E131),0,IF(E131=Answers!E131,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K131" t="str" cm="1">
+        <f t="array" ref="K131">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H131,_xlfn.SEQUENCE(1,LEN(H131),LEN(H131),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CTCACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCCTTTGCTCTGCCCG</v>
+      </c>
+      <c r="M131" t="str" cm="1">
+        <f t="array" ref="M131">MID(K131,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K131,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="25.5" customHeight="1">
       <c r="A132" s="1"/>
       <c r="B132" s="26">
         <f t="shared" si="10"/>
@@ -9519,17 +9680,27 @@
       <c r="D132" s="12">
         <v>7</v>
       </c>
-      <c r="E132" s="34"/>
+      <c r="E132" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="F132" s="10">
         <f>IF(ISBLANK(E132),0,IF(E132=Answers!E132,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K132" t="str" cm="1">
+        <f t="array" ref="K132">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H132,_xlfn.SEQUENCE(1,LEN(H132),LEN(H132),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CACTGCCTTTTGTCTGCCCAGTTTCACCAGAAGTAGGCCTCTTCCTGACAGGCAGCTGCACCACTGCCTGGCGCTGTGCCCTTCCTTTGCTCTGCCCGCT</v>
+      </c>
+      <c r="M132" t="str" cm="1">
+        <f t="array" ref="M132">MID(K132,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K132,4,999)),3)),3)</f>
+        <v>AAG</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="25.5" customHeight="1">
       <c r="A133" s="1"/>
       <c r="B133" s="26">
         <f t="shared" si="10"/>
@@ -9541,17 +9712,27 @@
       <c r="D133" s="12">
         <v>7</v>
       </c>
-      <c r="E133" s="34"/>
+      <c r="E133" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F133" s="10">
         <f>IF(ISBLANK(E133),0,IF(E133=Answers!E133,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133" s="1"/>
       <c r="H133" s="25" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K133" t="str" cm="1">
+        <f t="array" ref="K133">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H133,_xlfn.SEQUENCE(1,LEN(H133),LEN(H133),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GTGTATCACTGGTCCAGGAGCACTATGCTGGCAGAATCCCTTTGGTGCCTGATGGCCCTGCCTTCGTGGGAACAGAGGCTAAGGCTTTGAGTTACAGCTG</v>
+      </c>
+      <c r="M133" t="str" cm="1">
+        <f t="array" ref="M133">MID(K133,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K133,4,999)),3)),3)</f>
+        <v>GCC</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="25.5" customHeight="1">
       <c r="A134" s="1"/>
       <c r="B134" s="26">
         <f t="shared" si="10"/>
@@ -9563,17 +9744,27 @@
       <c r="D134" s="12">
         <v>7</v>
       </c>
-      <c r="E134" s="34"/>
+      <c r="E134" s="34" t="s">
+        <v>74</v>
+      </c>
       <c r="F134" s="10">
         <f>IF(ISBLANK(E134),0,IF(E134=Answers!E134,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" s="25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K134" t="str" cm="1">
+        <f t="array" ref="K134">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H134,_xlfn.SEQUENCE(1,LEN(H134),LEN(H134),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>TCACCTTTGTAGCAGGATCCCTGCAGACCAGGCCCATGACAAACACCGTCTCCAGCGGGCAGAGCAAAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCT</v>
+      </c>
+      <c r="M134" t="str" cm="1">
+        <f t="array" ref="M134">MID(K134,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K134,4,999)),3)),3)</f>
+        <v>TTG</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="25.5" customHeight="1">
       <c r="A135" s="1"/>
       <c r="B135" s="26">
         <f t="shared" si="10"/>
@@ -9585,17 +9776,27 @@
       <c r="D135" s="12">
         <v>7</v>
       </c>
-      <c r="E135" s="34"/>
+      <c r="E135" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F135" s="10">
         <f>IF(ISBLANK(E135),0,IF(E135=Answers!E135,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" s="25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K135" t="str" cm="1">
+        <f t="array" ref="K135">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H135,_xlfn.SEQUENCE(1,LEN(H135),LEN(H135),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>ACAAACACCGTCTCCAGCGGGCAGAGCAAAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCTGCCTGTCAGGAAGAGGCCTACTTCTGGTGAAACTGGGC</v>
+      </c>
+      <c r="M135" t="str" cm="1">
+        <f t="array" ref="M135">MID(K135,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K135,4,999)),3)),3)</f>
+        <v>TGG</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="25.5" customHeight="1">
       <c r="A136" s="1"/>
       <c r="B136" s="26">
         <f t="shared" si="10"/>
@@ -9607,17 +9808,27 @@
       <c r="D136" s="12">
         <v>7</v>
       </c>
-      <c r="E136" s="34"/>
+      <c r="E136" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F136" s="10">
         <f>IF(ISBLANK(E136),0,IF(E136=Answers!E136,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G136" s="1"/>
       <c r="H136" s="25" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K136" t="str" cm="1">
+        <f t="array" ref="K136">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H136,_xlfn.SEQUENCE(1,LEN(H136),LEN(H136),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CCGTCTCCAGCGGGCAGAGCAAAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCTGCCTGTCAGGAAGAGGCCTACTTCTGGTGAAACTGGGCAGACAAA</v>
+      </c>
+      <c r="M136" t="str" cm="1">
+        <f t="array" ref="M136">MID(K136,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K136,4,999)),3)),3)</f>
+        <v>TGG</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="25.5" customHeight="1">
       <c r="A137" s="1"/>
       <c r="B137" s="26">
         <f t="shared" si="10"/>
@@ -9629,17 +9840,27 @@
       <c r="D137" s="12">
         <v>7</v>
       </c>
-      <c r="E137" s="34"/>
+      <c r="E137" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F137" s="10">
         <f>IF(ISBLANK(E137),0,IF(E137=Answers!E137,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K137" t="str" cm="1">
+        <f t="array" ref="K137">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H137,_xlfn.SEQUENCE(1,LEN(H137),LEN(H137),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>AAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCTGCCTGTCAGGAAGAGGCCTACTTCTGGTGAAACTGGGCAGACAAAAGGCAGTGAGAAATGTGATCT</v>
+      </c>
+      <c r="M137" t="str" cm="1">
+        <f t="array" ref="M137">MID(K137,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K137,4,999)),3)),3)</f>
+        <v>TGG</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="25.5" customHeight="1">
       <c r="A138" s="1"/>
       <c r="B138" s="26">
         <f t="shared" si="10"/>
@@ -9651,17 +9872,27 @@
       <c r="D138" s="12">
         <v>7</v>
       </c>
-      <c r="E138" s="34"/>
+      <c r="E138" s="34" t="s">
+        <v>62</v>
+      </c>
       <c r="F138" s="10">
         <f>IF(ISBLANK(E138),0,IF(E138=Answers!E138,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G138" s="1"/>
       <c r="H138" s="25" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="25.5" customHeight="1">
+      <c r="K138" t="str" cm="1">
+        <f t="array" ref="K138">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H138,_xlfn.SEQUENCE(1,LEN(H138),LEN(H138),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>GGGCCCCTGCCCATCCGTGAGATCTTCCCAGGGCAGCTCCCCTCTGTGGAATCCAATCTGTCTTCCATCCTGCGTGGCCGAGGGCCAGGCTTCTCACTGG</v>
+      </c>
+      <c r="M138" t="str" cm="1">
+        <f t="array" ref="M138">MID(K138,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K138,4,999)),3)),3)</f>
+        <v>CCG</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="25.5" customHeight="1">
       <c r="A139" s="1"/>
       <c r="B139" s="26">
         <f t="shared" si="10"/>
@@ -9673,17 +9904,27 @@
       <c r="D139" s="12">
         <v>7</v>
       </c>
-      <c r="E139" s="34"/>
+      <c r="E139" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="F139" s="10">
         <f>IF(ISBLANK(E139),0,IF(E139=Answers!E139,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" s="25" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="15" customHeight="1">
+      <c r="K139" t="str" cm="1">
+        <f t="array" ref="K139">_xlfn.CONCAT(_xlfn.XLOOKUP(MID(H139,_xlfn.SEQUENCE(1,LEN(H139),LEN(H139),-1),1),$J$109:$J$112,$K$109:$K$112))</f>
+        <v>CACCGTCTCCAGCGGACAGAGCAAAGGAAGGGCACAGCGCCAGGCAGTGGTGCAGCTGCCTGTCAGGAAGAGGCCTACTTCTGGTGAAACTGGGCAGACA</v>
+      </c>
+      <c r="M139" t="str" cm="1">
+        <f t="array" ref="M139">MID(K139,MIN(_xlfn.TOCOL(SEARCH(_nStop,MID(K139,4,999)),3)),3)</f>
+        <v>TGG</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="15" customHeight="1">
       <c r="A140" s="1"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -9693,7 +9934,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="4"/>
     </row>
-    <row r="141" spans="1:8" ht="15" customHeight="1">
+    <row r="141" spans="1:13" ht="15" customHeight="1">
       <c r="A141" s="1"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -9703,7 +9944,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="4"/>
     </row>
-    <row r="142" spans="1:8" ht="24.75" customHeight="1">
+    <row r="142" spans="1:13" ht="24.75" customHeight="1">
       <c r="A142" s="1"/>
       <c r="B142" s="18" t="s">
         <v>117</v>
@@ -9719,7 +9960,7 @@
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
     </row>
-    <row r="143" spans="1:8" ht="14.25" customHeight="1">
+    <row r="143" spans="1:13" ht="14.25" customHeight="1">
       <c r="A143" s="1"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -9729,7 +9970,7 @@
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
     </row>
-    <row r="144" spans="1:8" ht="14.25" customHeight="1">
+    <row r="144" spans="1:13" ht="14.25" customHeight="1">
       <c r="A144" s="1"/>
       <c r="B144" s="3" t="s">
         <v>120</v>
@@ -21012,10 +21253,10 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="47"/>
-      <c r="B2" s="201" t="s">
+      <c r="B2" s="194" t="s">
         <v>1019</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="196" t="s">
         <v>1020</v>
       </c>
       <c r="D2" s="180"/>
@@ -21025,7 +21266,7 @@
       <c r="H2" s="180"/>
       <c r="I2" s="180"/>
       <c r="J2" s="181"/>
-      <c r="K2" s="188" t="s">
+      <c r="K2" s="197" t="s">
         <v>1021</v>
       </c>
       <c r="L2" s="48"/>
@@ -21033,30 +21274,30 @@
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="47"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="190" t="s">
+      <c r="B3" s="195"/>
+      <c r="C3" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="191"/>
-      <c r="E3" s="190" t="s">
+      <c r="D3" s="200"/>
+      <c r="E3" s="199" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="191"/>
-      <c r="G3" s="192" t="s">
+      <c r="F3" s="200"/>
+      <c r="G3" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="193"/>
-      <c r="I3" s="192" t="s">
+      <c r="H3" s="202"/>
+      <c r="I3" s="201" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="193"/>
-      <c r="K3" s="189"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="198"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
       <c r="A4" s="47"/>
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="187" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="53" t="s">
@@ -21091,7 +21332,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="47"/>
-      <c r="B5" s="195"/>
+      <c r="B5" s="188"/>
       <c r="C5" s="62" t="s">
         <v>1028</v>
       </c>
@@ -21124,7 +21365,7 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="47"/>
-      <c r="B6" s="195"/>
+      <c r="B6" s="188"/>
       <c r="C6" s="70" t="s">
         <v>68</v>
       </c>
@@ -21157,7 +21398,7 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="47"/>
-      <c r="B7" s="196"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="76" t="s">
         <v>74</v>
       </c>
@@ -21190,7 +21431,7 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="47"/>
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="190" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="84" t="s">
@@ -21226,7 +21467,7 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="47"/>
-      <c r="B9" s="198"/>
+      <c r="B9" s="191"/>
       <c r="C9" s="70" t="s">
         <v>1047</v>
       </c>
@@ -21259,7 +21500,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="47"/>
-      <c r="B10" s="198"/>
+      <c r="B10" s="191"/>
       <c r="C10" s="70" t="s">
         <v>1050</v>
       </c>
@@ -21292,7 +21533,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="47"/>
-      <c r="B11" s="199"/>
+      <c r="B11" s="192"/>
       <c r="C11" s="76" t="s">
         <v>66</v>
       </c>
@@ -21325,7 +21566,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="47"/>
-      <c r="B12" s="197" t="s">
+      <c r="B12" s="190" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="106" t="s">
@@ -21361,7 +21602,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="47"/>
-      <c r="B13" s="198"/>
+      <c r="B13" s="191"/>
       <c r="C13" s="112" t="s">
         <v>1064</v>
       </c>
@@ -21394,7 +21635,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="47"/>
-      <c r="B14" s="198"/>
+      <c r="B14" s="191"/>
       <c r="C14" s="112" t="s">
         <v>1067</v>
       </c>
@@ -21427,7 +21668,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="47"/>
-      <c r="B15" s="199"/>
+      <c r="B15" s="192"/>
       <c r="C15" s="122" t="s">
         <v>1072</v>
       </c>
@@ -21460,7 +21701,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="47"/>
-      <c r="B16" s="197" t="s">
+      <c r="B16" s="190" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="130" t="s">
@@ -21496,7 +21737,7 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="47"/>
-      <c r="B17" s="198"/>
+      <c r="B17" s="191"/>
       <c r="C17" s="138" t="s">
         <v>1084</v>
       </c>
@@ -21529,7 +21770,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="47"/>
-      <c r="B18" s="198"/>
+      <c r="B18" s="191"/>
       <c r="C18" s="138" t="s">
         <v>1087</v>
       </c>
@@ -21562,7 +21803,7 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="47"/>
-      <c r="B19" s="200"/>
+      <c r="B19" s="193"/>
       <c r="C19" s="148" t="s">
         <v>1092</v>
       </c>
@@ -25434,17 +25675,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>